<commit_message>
RK3588 SBC Specifications updated.
</commit_message>
<xml_diff>
--- a/04 RK3588 SBC Specifications.xlsx
+++ b/04 RK3588 SBC Specifications.xlsx
@@ -972,15 +972,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>828040</xdr:colOff>
+      <xdr:colOff>55880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>86995</xdr:rowOff>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2413000</xdr:colOff>
+      <xdr:colOff>1193800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>2561590</xdr:rowOff>
+      <xdr:rowOff>2166620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -997,8 +997,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="828040" y="14280515"/>
-          <a:ext cx="3129280" cy="2474595"/>
+          <a:off x="55880" y="14237970"/>
+          <a:ext cx="2682240" cy="2122170"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1010,15 +1010,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2938145</xdr:colOff>
+      <xdr:colOff>1290955</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6197600</xdr:colOff>
+      <xdr:colOff>4118610</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>2558415</xdr:rowOff>
+      <xdr:rowOff>2171700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1035,8 +1035,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4482465" y="14288770"/>
-          <a:ext cx="3259455" cy="2463165"/>
+          <a:off x="2835275" y="14228445"/>
+          <a:ext cx="2827655" cy="2136775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4105275</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7160895</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>2224405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3" descr="RK3588_size"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5649595" y="14218920"/>
+          <a:ext cx="3055620" cy="2199005"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1308,8 +1346,8 @@
   <sheetPr/>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -1562,7 +1600,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" ht="204" customHeight="1" spans="1:3">
+    <row r="29" ht="178" customHeight="1" spans="1:3">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>

</xml_diff>